<commit_message>
Had workshop afio not use mmaps except for large files. Updated graphs.
</commit_message>
<xml_diff>
--- a/doc/workshop.xlsx
+++ b/doc/workshop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="300" windowWidth="17085" windowHeight="15840"/>
+    <workbookView xWindow="4515" yWindow="75" windowWidth="17085" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -664,11 +664,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77340672"/>
-        <c:axId val="77366400"/>
+        <c:axId val="164779520"/>
+        <c:axId val="164814848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77340672"/>
+        <c:axId val="164779520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -693,14 +693,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77366400"/>
+        <c:crossAx val="164814848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77366400"/>
+        <c:axId val="164814848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120000"/>
@@ -709,7 +709,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77340672"/>
+        <c:crossAx val="164779520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -722,7 +722,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -984,55 +984,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>3776.79</c:v>
+                  <c:v>3387.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7479.21</c:v>
+                  <c:v>6071.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9288.0300000000007</c:v>
+                  <c:v>8642.2000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11322.6</c:v>
+                  <c:v>10837.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17106</c:v>
+                  <c:v>22987.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20707.3</c:v>
+                  <c:v>24311.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21275.200000000001</c:v>
+                  <c:v>28557.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22651</c:v>
+                  <c:v>26149.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23152</c:v>
+                  <c:v>25437</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23628.1</c:v>
+                  <c:v>25824</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23370.9</c:v>
+                  <c:v>27736.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22498.5</c:v>
+                  <c:v>25773.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23550.3</c:v>
+                  <c:v>27289.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22593.599999999999</c:v>
+                  <c:v>27736.9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24511</c:v>
+                  <c:v>28423.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25785.7</c:v>
+                  <c:v>30949.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25701.3</c:v>
+                  <c:v>30518.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,7 +1152,7 @@
                   <c:v>40828.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>85196.4</c:v>
+                  <c:v>66621.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>51057.599999999999</c:v>
@@ -1260,66 +1260,66 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>17936.900000000001</c:v>
+                  <c:v>116.077</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3100.3</c:v>
+                  <c:v>1689.37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14823.4</c:v>
+                  <c:v>1035.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5761.34</c:v>
+                  <c:v>1171.3800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3890.78</c:v>
+                  <c:v>1933.59</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3305.95</c:v>
+                  <c:v>4002.57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9371.4599999999991</c:v>
+                  <c:v>12459.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16558.5</c:v>
+                  <c:v>11459.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22656.3</c:v>
+                  <c:v>17425.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27204.7</c:v>
+                  <c:v>20406.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19999.8</c:v>
+                  <c:v>19320.900000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19473.900000000001</c:v>
+                  <c:v>18141.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23042.2</c:v>
+                  <c:v>17596.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20346.2</c:v>
+                  <c:v>19391.099999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20945.3</c:v>
+                  <c:v>19915.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20707.8</c:v>
+                  <c:v>19522.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20670.900000000001</c:v>
+                  <c:v>20294.599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="111795200"/>
-        <c:axId val="111838336"/>
+        <c:axId val="163006336"/>
+        <c:axId val="163020800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111795200"/>
+        <c:axId val="163006336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,14 +1344,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111838336"/>
+        <c:crossAx val="163020800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111838336"/>
+        <c:axId val="163020800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,7 +1359,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111795200"/>
+        <c:crossAx val="163006336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1372,7 +1372,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1731,7 +1731,7 @@
   <dimension ref="A2:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2068,13 +2068,13 @@
         <v>7350.51</v>
       </c>
       <c r="C22">
-        <v>3776.79</v>
+        <v>3387.51</v>
       </c>
       <c r="D22">
         <v>197.02500000000001</v>
       </c>
       <c r="E22">
-        <v>17936.900000000001</v>
+        <v>116.077</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2085,13 +2085,13 @@
         <v>21632.799999999999</v>
       </c>
       <c r="C23">
-        <v>7479.21</v>
+        <v>6071.04</v>
       </c>
       <c r="D23">
         <v>302.95299999999997</v>
       </c>
       <c r="E23">
-        <v>3100.3</v>
+        <v>1689.37</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2102,13 +2102,13 @@
         <v>43680.5</v>
       </c>
       <c r="C24">
-        <v>9288.0300000000007</v>
+        <v>8642.2000000000007</v>
       </c>
       <c r="D24">
         <v>645.16700000000003</v>
       </c>
       <c r="E24">
-        <v>14823.4</v>
+        <v>1035.77</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2119,13 +2119,13 @@
         <v>69577.3</v>
       </c>
       <c r="C25">
-        <v>11322.6</v>
+        <v>10837.9</v>
       </c>
       <c r="D25">
         <v>1215.71</v>
       </c>
       <c r="E25">
-        <v>5761.34</v>
+        <v>1171.3800000000001</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2136,13 +2136,13 @@
         <v>67516</v>
       </c>
       <c r="C26">
-        <v>17106</v>
+        <v>22987.7</v>
       </c>
       <c r="D26">
         <v>2062.63</v>
       </c>
       <c r="E26">
-        <v>3890.78</v>
+        <v>1933.59</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2153,13 +2153,13 @@
         <v>102700</v>
       </c>
       <c r="C27">
-        <v>20707.3</v>
+        <v>24311.1</v>
       </c>
       <c r="D27">
         <v>4815.63</v>
       </c>
       <c r="E27">
-        <v>3305.95</v>
+        <v>4002.57</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2170,13 +2170,13 @@
         <v>114231</v>
       </c>
       <c r="C28">
-        <v>21275.200000000001</v>
+        <v>28557.599999999999</v>
       </c>
       <c r="D28">
         <v>9579.2900000000009</v>
       </c>
       <c r="E28">
-        <v>9371.4599999999991</v>
+        <v>12459.9</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2187,13 +2187,13 @@
         <v>113460</v>
       </c>
       <c r="C29">
-        <v>22651</v>
+        <v>26149.200000000001</v>
       </c>
       <c r="D29">
         <v>18798.400000000001</v>
       </c>
       <c r="E29">
-        <v>16558.5</v>
+        <v>11459.6</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2204,13 +2204,13 @@
         <v>72034.8</v>
       </c>
       <c r="C30">
-        <v>23152</v>
+        <v>25437</v>
       </c>
       <c r="D30">
         <v>35731.4</v>
       </c>
       <c r="E30">
-        <v>22656.3</v>
+        <v>17425.3</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2221,13 +2221,13 @@
         <v>69885.899999999994</v>
       </c>
       <c r="C31">
-        <v>23628.1</v>
+        <v>25824</v>
       </c>
       <c r="D31">
         <v>40828.5</v>
       </c>
       <c r="E31">
-        <v>27204.7</v>
+        <v>20406.2</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2238,13 +2238,13 @@
         <v>95933.1</v>
       </c>
       <c r="C32">
-        <v>23370.9</v>
+        <v>27736.2</v>
       </c>
       <c r="D32">
-        <v>85196.4</v>
+        <v>66621.8</v>
       </c>
       <c r="E32">
-        <v>19999.8</v>
+        <v>19320.900000000001</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2255,13 +2255,13 @@
         <v>81844.2</v>
       </c>
       <c r="C33">
-        <v>22498.5</v>
+        <v>25773.4</v>
       </c>
       <c r="D33">
         <v>51057.599999999999</v>
       </c>
       <c r="E33">
-        <v>19473.900000000001</v>
+        <v>18141.8</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2272,13 +2272,13 @@
         <v>92156.2</v>
       </c>
       <c r="C34">
-        <v>23550.3</v>
+        <v>27289.9</v>
       </c>
       <c r="D34">
         <v>65586.899999999994</v>
       </c>
       <c r="E34">
-        <v>23042.2</v>
+        <v>17596.7</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2289,13 +2289,13 @@
         <v>94505.2</v>
       </c>
       <c r="C35">
-        <v>22593.599999999999</v>
+        <v>27736.9</v>
       </c>
       <c r="D35">
         <v>64637.9</v>
       </c>
       <c r="E35">
-        <v>20346.2</v>
+        <v>19391.099999999999</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2306,13 +2306,13 @@
         <v>89699.4</v>
       </c>
       <c r="C36">
-        <v>24511</v>
+        <v>28423.3</v>
       </c>
       <c r="D36">
         <v>63261.9</v>
       </c>
       <c r="E36">
-        <v>20945.3</v>
+        <v>19915.2</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2323,13 +2323,13 @@
         <v>76715.3</v>
       </c>
       <c r="C37">
-        <v>25785.7</v>
+        <v>30949.5</v>
       </c>
       <c r="D37">
         <v>58911.5</v>
       </c>
       <c r="E37">
-        <v>20707.8</v>
+        <v>19522.8</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2340,13 +2340,13 @@
         <v>107904</v>
       </c>
       <c r="C38">
-        <v>25701.3</v>
+        <v>30518.2</v>
       </c>
       <c r="D38">
         <v>59622.3</v>
       </c>
       <c r="E38">
-        <v>20670.900000000001</v>
+        <v>20294.599999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished next workshop section.
</commit_message>
<xml_diff>
--- a/doc/workshop.xlsx
+++ b/doc/workshop.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="75" windowWidth="17085" windowHeight="15840"/>
+    <workbookView xWindow="4515" yWindow="75" windowWidth="17085" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Naive" sheetId="1" r:id="rId1"/>
+    <sheet name="Atomic" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Items</t>
   </si>
@@ -31,6 +31,24 @@
   </si>
   <si>
     <t>ext4 AFIO</t>
+  </si>
+  <si>
+    <t>NTFS</t>
+  </si>
+  <si>
+    <t>ext4</t>
+  </si>
+  <si>
+    <t>NTFS Inserts/sec</t>
+  </si>
+  <si>
+    <t>NTFS Lookups/sec</t>
+  </si>
+  <si>
+    <t>ext4 Inserts/sec</t>
+  </si>
+  <si>
+    <t>ext4 Lookups/sec</t>
   </si>
 </sst>
 </file>
@@ -116,7 +134,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Naive!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -130,7 +148,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$19</c:f>
+              <c:f>Naive!$A$3:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -190,7 +208,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$19</c:f>
+              <c:f>Naive!$B$3:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -254,7 +272,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Naive!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -268,7 +286,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$19</c:f>
+              <c:f>Naive!$A$3:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -328,7 +346,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$19</c:f>
+              <c:f>Naive!$C$3:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -392,7 +410,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Naive!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -406,7 +424,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$19</c:f>
+              <c:f>Naive!$A$3:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -466,7 +484,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$19</c:f>
+              <c:f>Naive!$D$3:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -530,7 +548,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Naive!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -544,7 +562,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$19</c:f>
+              <c:f>Naive!$A$3:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -604,7 +622,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$19</c:f>
+              <c:f>Naive!$E$3:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -664,11 +682,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="164779520"/>
-        <c:axId val="164814848"/>
+        <c:axId val="158098944"/>
+        <c:axId val="158130176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="164779520"/>
+        <c:axId val="158098944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -693,23 +711,22 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164814848"/>
+        <c:crossAx val="158130176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164814848"/>
+        <c:axId val="158130176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="120000"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164779520"/>
+        <c:crossAx val="158098944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -722,7 +739,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -767,7 +784,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Naive!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -781,7 +798,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$22:$A$38</c:f>
+              <c:f>Naive!$A$22:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -841,7 +858,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$22:$B$38</c:f>
+              <c:f>Naive!$B$22:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -905,7 +922,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Naive!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -919,7 +936,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$22:$A$38</c:f>
+              <c:f>Naive!$A$22:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -979,7 +996,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$22:$C$38</c:f>
+              <c:f>Naive!$C$22:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1043,7 +1060,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Naive!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1057,7 +1074,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$22:$A$38</c:f>
+              <c:f>Naive!$A$22:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1117,7 +1134,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$22:$D$38</c:f>
+              <c:f>Naive!$D$22:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1181,7 +1198,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Naive!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1195,7 +1212,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$22:$A$38</c:f>
+              <c:f>Naive!$A$22:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1255,7 +1272,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$22:$E$38</c:f>
+              <c:f>Naive!$E$22:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1315,11 +1332,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="163006336"/>
-        <c:axId val="163020800"/>
+        <c:axId val="157759360"/>
+        <c:axId val="157777920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163006336"/>
+        <c:axId val="157759360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,14 +1361,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163020800"/>
+        <c:crossAx val="157777920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163020800"/>
+        <c:axId val="157777920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,7 +1376,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163006336"/>
+        <c:crossAx val="157759360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1372,7 +1389,1044 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-IE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Atomic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> key-value BLOB store insertions/sec</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>NTFS atomic</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Atomic!$A$3:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Atomic!$B$3:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>629.69600000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1353.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2105.9699999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1579.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1044.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>743.24900000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>488.87799999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>738.899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>820.67100000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>817.08699999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>788.27200000000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>727.21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>731.60400000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>726.09</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>724.53300000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>721.61900000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>719.62800000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>NTFS naive</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Naive!$C$3:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>330.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>795.15899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1440.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1701.55</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2415.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2536.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2925.23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2935.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2952.22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3462</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3233.92</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3009.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2766.01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2493.33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2546.77</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2510.1799999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2489.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ext4 atomic</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Atomic!$A$3:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Atomic!$D$3:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>98.696299999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>217.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>514.90700000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>917.28800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2641.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2461.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3584.31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3932.26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2981.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2675.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2656.82</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2578.2800000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2638.28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2495.19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2202.87</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1847.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1653.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>ext4 naive</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Naive!$E$3:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>87.369200000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>174.13300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>520.43299999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1479.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1691.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3006.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4539.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7147.93</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10270.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11171.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11667.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11382.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11239.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10890.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10682.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10499.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10725.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="158286592"/>
+        <c:axId val="75003008"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="158286592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Items</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75003008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75003008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12000"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="158286592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-IE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Atomic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> key-value BLOB store lookups/sec</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>NTFS atomic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Atomic!$A$3:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Atomic!$C$3:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>3616.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7471.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11016.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11097.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17132.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24689.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27245.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30401.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31283.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31887.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32322.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32490.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29799.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32554.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30420</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32124.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32008.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>NTFS naive</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Naive!$C$22:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>3387.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6071.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8642.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10837.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22987.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24311.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28557.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26149.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25437</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25824</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27736.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25773.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27289.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27736.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28423.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30949.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30518.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ext4 atomic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="9BBB59">
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Atomic!$A$3:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Atomic!$E$3:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>395.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600.01900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1045.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2311.1799999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4101.9399999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7645.34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12203</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17770.099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18042.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16405.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17058</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17054.900000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18080.900000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17809</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18574.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18142.099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>ext4 naive</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Naive!$E$22:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>116.077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1689.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1035.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1171.3800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1933.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4002.57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12459.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11459.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17425.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20406.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19320.900000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18141.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17596.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19391.099999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19915.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19522.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20294.599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="108086400"/>
+        <c:axId val="108088320"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="108086400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Items</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108088320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="108088320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108086400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1426,6 +2480,71 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>256800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>247275</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>189675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1730,8 +2849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2357,13 +3476,331 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>629.69600000000003</v>
+      </c>
+      <c r="C3">
+        <v>3616.92</v>
+      </c>
+      <c r="D3">
+        <v>98.696299999999994</v>
+      </c>
+      <c r="E3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1353.66</v>
+      </c>
+      <c r="C4">
+        <v>7471.02</v>
+      </c>
+      <c r="D4">
+        <v>217.82</v>
+      </c>
+      <c r="E4">
+        <v>395.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2105.9699999999998</v>
+      </c>
+      <c r="C5">
+        <v>11016.9</v>
+      </c>
+      <c r="D5">
+        <v>514.90700000000004</v>
+      </c>
+      <c r="E5">
+        <v>600.01900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1579.48</v>
+      </c>
+      <c r="C6">
+        <v>11097.4</v>
+      </c>
+      <c r="D6">
+        <v>917.28800000000001</v>
+      </c>
+      <c r="E6">
+        <v>1045.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1044.96</v>
+      </c>
+      <c r="C7">
+        <v>17132.8</v>
+      </c>
+      <c r="D7">
+        <v>2641.1</v>
+      </c>
+      <c r="E7">
+        <v>2311.1799999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>743.24900000000002</v>
+      </c>
+      <c r="C8">
+        <v>24689.8</v>
+      </c>
+      <c r="D8">
+        <v>2461.35</v>
+      </c>
+      <c r="E8">
+        <v>4101.9399999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>64</v>
+      </c>
+      <c r="B9">
+        <v>488.87799999999999</v>
+      </c>
+      <c r="C9">
+        <v>27245.200000000001</v>
+      </c>
+      <c r="D9">
+        <v>3584.31</v>
+      </c>
+      <c r="E9">
+        <v>7645.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>128</v>
+      </c>
+      <c r="B10">
+        <v>738.899</v>
+      </c>
+      <c r="C10">
+        <v>30401.200000000001</v>
+      </c>
+      <c r="D10">
+        <v>3932.26</v>
+      </c>
+      <c r="E10">
+        <v>12203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>256</v>
+      </c>
+      <c r="B11">
+        <v>820.67100000000005</v>
+      </c>
+      <c r="C11">
+        <v>31283.7</v>
+      </c>
+      <c r="D11">
+        <v>2981.39</v>
+      </c>
+      <c r="E11">
+        <v>17770.099999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>512</v>
+      </c>
+      <c r="B12">
+        <v>817.08699999999999</v>
+      </c>
+      <c r="C12">
+        <v>31887.4</v>
+      </c>
+      <c r="D12">
+        <v>2675.25</v>
+      </c>
+      <c r="E12">
+        <v>18042.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>1024</v>
+      </c>
+      <c r="B13">
+        <v>788.27200000000005</v>
+      </c>
+      <c r="C13">
+        <v>32322.9</v>
+      </c>
+      <c r="D13">
+        <v>2656.82</v>
+      </c>
+      <c r="E13">
+        <v>16405.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>2048</v>
+      </c>
+      <c r="B14">
+        <v>727.21</v>
+      </c>
+      <c r="C14">
+        <v>32490.2</v>
+      </c>
+      <c r="D14">
+        <v>2578.2800000000002</v>
+      </c>
+      <c r="E14">
+        <v>17058</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>4096</v>
+      </c>
+      <c r="B15">
+        <v>731.60400000000004</v>
+      </c>
+      <c r="C15">
+        <v>29799.1</v>
+      </c>
+      <c r="D15">
+        <v>2638.28</v>
+      </c>
+      <c r="E15">
+        <v>17054.900000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>8192</v>
+      </c>
+      <c r="B16">
+        <v>726.09</v>
+      </c>
+      <c r="C16">
+        <v>32554.400000000001</v>
+      </c>
+      <c r="D16">
+        <v>2495.19</v>
+      </c>
+      <c r="E16">
+        <v>18080.900000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16384</v>
+      </c>
+      <c r="B17">
+        <v>724.53300000000002</v>
+      </c>
+      <c r="C17">
+        <v>30420</v>
+      </c>
+      <c r="D17">
+        <v>2202.87</v>
+      </c>
+      <c r="E17">
+        <v>17809</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>32768</v>
+      </c>
+      <c r="B18">
+        <v>721.61900000000003</v>
+      </c>
+      <c r="C18">
+        <v>32124.9</v>
+      </c>
+      <c r="D18">
+        <v>1847.04</v>
+      </c>
+      <c r="E18">
+        <v>18574.400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>65536</v>
+      </c>
+      <c r="B19">
+        <v>719.62800000000004</v>
+      </c>
+      <c r="C19">
+        <v>32008.7</v>
+      </c>
+      <c r="D19">
+        <v>1653.16</v>
+      </c>
+      <c r="E19">
+        <v>18142.099999999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>